<commit_message>
Add task in `game-theory`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/game-theory/Бронников ПМ-1901 - Анализ платёжной матрица.xlsx
+++ b/3-course-6-semester/game-theory/Бронников ПМ-1901 - Анализ платёжной матрица.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\game-theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA1DBDB-CDA8-418C-889B-23684D8A19C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68F8138-90C8-42CB-8ABD-56F38599D2E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="4560" windowWidth="20730" windowHeight="11310" xr2:uid="{014FD5D8-6377-47C8-8ED7-EB12F91E9EBA}"/>
+    <workbookView xWindow="3495" yWindow="6750" windowWidth="15375" windowHeight="8085" xr2:uid="{014FD5D8-6377-47C8-8ED7-EB12F91E9EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Матрица" sheetId="1" r:id="rId1"/>
@@ -583,23 +583,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -610,11 +598,11 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -628,14 +616,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -661,55 +661,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2724,10 +2675,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -3028,7 +2975,7 @@
   <dimension ref="A2:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X8" sqref="X8"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3039,22 +2986,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
     </row>
     <row r="3" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
@@ -3090,10 +3037,10 @@
       <c r="L3" s="10">
         <v>10</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="17"/>
+      <c r="O3" s="28"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="10">
@@ -3565,10 +3512,10 @@
     </row>
     <row r="16" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:19" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="16"/>
+      <c r="B17" s="27"/>
       <c r="C17" s="11">
         <f>MAX(C4:C15)</f>
         <v>10</v>
@@ -3605,57 +3552,57 @@
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="L17" s="30">
+      <c r="L17" s="21">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="19" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="O19" s="18" t="s">
+      <c r="O19" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="16">
         <f>MAX(N4:N15)</f>
         <v>3</v>
       </c>
-      <c r="Q19" s="20" t="s">
+      <c r="Q19" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="R19" s="20"/>
-      <c r="S19" s="21">
+      <c r="R19" s="29"/>
+      <c r="S19" s="17">
         <f>MATCH(P19,N4:N15,0)</f>
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="O20" s="22" t="s">
+      <c r="O20" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="19">
         <f>MIN(C17:L17)</f>
         <v>3</v>
       </c>
-      <c r="Q20" s="24" t="s">
+      <c r="Q20" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="R20" s="24"/>
-      <c r="S20" s="25">
+      <c r="R20" s="30"/>
+      <c r="S20" s="20">
         <f>MATCH(P20,C17:L17)</f>
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="O21" s="26" t="s">
+      <c r="O21" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="28" t="str">
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="24" t="str">
         <f>IF(P19=P20,"ДА","НЕТ")</f>
         <v>ДА</v>
       </c>
-      <c r="S21" s="29"/>
+      <c r="S21" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3668,26 +3615,26 @@
     <mergeCell ref="Q20:R20"/>
   </mergeCells>
   <conditionalFormatting sqref="N4:N15">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>$N4=$P$19</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17:L17">
-    <cfRule type="expression" dxfId="10" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>C$17=$P$20</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:L15">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>$C$17=$N$4</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>AND($C$4=$C$17, $C$4=$N$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(C4=$C17,C4=N$4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(C4=C$17,C4=$N4)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>